<commit_message>
Support units when ingesting wealth characteristics - see HEA-130
This MR also updates the ingestion pipeline to support various
other changes resulting from the Dakar validation workshop,
such as additional metadata like the data collection dates in
the LivelihoodZoneBaseline, and the renaming of `source` to
`reference_type` in `WealthGroupCharacteristicValue`
</commit_message>
<xml_diff>
--- a/apps/baseline/tests/metadata.xlsx
+++ b/apps/baseline/tests/metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">bss_path</t>
   </si>
@@ -52,6 +52,15 @@
     <t xml:space="preserve">valid_to_date</t>
   </si>
   <si>
+    <t xml:space="preserve">data_collection_start_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_collection_end_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publication_date</t>
+  </si>
+  <si>
     <t xml:space="preserve">tests/bss.xlsx</t>
   </si>
   <si>
@@ -62,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">FEWS NET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kasungu Lilongwe Plains </t>
   </si>
   <si>
     <t xml:space="preserve">Agropastoral</t>
@@ -80,6 +92,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -101,6 +114,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,13 +159,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -175,19 +193,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="24.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -221,33 +243,45 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="n">
         <v>41730</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="3" t="n">
         <v>42125</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>42156</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="3" t="n">
         <v>45809</v>
       </c>
     </row>

</xml_diff>